<commit_message>
Refactor symbol conversion: Remove redundant dependencies, improve `OptionSymbolConverter` docs, and enhance modularity with `OptionFormat`.
</commit_message>
<xml_diff>
--- a/EbfTrading/resources/specs/Use Cases.xlsx
+++ b/EbfTrading/resources/specs/Use Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finge\PycharmProjects\EbfTrading\resources\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CE4DA7-DF91-4AC9-8504-4AD0FBAAD799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54ECAAB9-C108-40F3-9856-F75053B6CEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00FE1F8B-6966-4E31-B613-544183EFD1DF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00FE1F8B-6966-4E31-B613-544183EFD1DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Unfilled LMT Order" sheetId="3" r:id="rId1"/>
@@ -654,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F6A6F6-B901-4DAE-A860-009525B4BCE3}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -963,6 +963,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -970,7 +971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC13F5D-6787-4A2E-8687-321A6306D415}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1657,8 +1658,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>